<commit_message>
squashed super gnarly bug with target create
Did a lot of clean up in the process.
Discovered bug in indictor manager with displaying system indicator during error.
</commit_message>
<xml_diff>
--- a/Design/json_overhead.xlsx
+++ b/Design/json_overhead.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsasala/Development/Aquarius/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34DFE03-F58A-F348-B01E-EBBC291F6A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C15C613-F5E1-0B45-89FA-8AE33DEDB3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17380" yWindow="4720" windowWidth="28040" windowHeight="17440" xr2:uid="{24EE9256-B69D-0E43-93A7-E6DCB16B0368}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -706,7 +706,7 @@
       </c>
       <c r="F18">
         <f>C18*C16+(C16-1)+9</f>
-        <v>96</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
       </c>
       <c r="C19">
         <f>C18*C16+(C16-1)*B9</f>
-        <v>87</v>
+        <v>439</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
@@ -727,7 +727,7 @@
       </c>
       <c r="C20">
         <f>C19+F2+B11</f>
-        <v>94</v>
+        <v>446</v>
       </c>
       <c r="D20" t="s">
         <v>23</v>
@@ -739,7 +739,7 @@
       </c>
       <c r="C21">
         <f>C20+B12</f>
-        <v>96</v>
+        <v>448</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>

</xml_diff>